<commit_message>
Change inlet multiplier to 2.5
</commit_message>
<xml_diff>
--- a/Inlet_calculations.xlsx
+++ b/Inlet_calculations.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\modeling\HEC-HMS\Bloomingdale\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="12300"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -242,6 +247,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -289,7 +297,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -324,7 +332,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -535,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F33" sqref="F5:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +563,7 @@
         <v>42</v>
       </c>
       <c r="J2" s="1">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="L2" t="s">
         <v>43</v>
@@ -602,11 +610,11 @@
       </c>
       <c r="E5" s="4">
         <f>D5*$J$2*$N$2*(1-$Q$2/100)</f>
-        <v>37.799999999999997</v>
+        <v>62.999999999999993</v>
       </c>
       <c r="F5" s="4">
         <f>E5*1.54723</f>
-        <v>58.485293999999996</v>
+        <v>97.475489999999994</v>
       </c>
     </row>
     <row r="6" spans="3:18" x14ac:dyDescent="0.25">
@@ -637,11 +645,11 @@
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>102.06</v>
+        <v>170.1</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="1"/>
-        <v>157.91029380000001</v>
+        <v>263.18382300000002</v>
       </c>
     </row>
     <row r="8" spans="3:18" x14ac:dyDescent="0.25">
@@ -653,11 +661,11 @@
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>60.48</v>
+        <v>100.8</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="1"/>
-        <v>93.576470400000005</v>
+        <v>155.96078400000002</v>
       </c>
     </row>
     <row r="9" spans="3:18" x14ac:dyDescent="0.25">
@@ -669,11 +677,11 @@
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>88.83</v>
+        <v>148.04999999999998</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="1"/>
-        <v>137.4404409</v>
+        <v>229.06740149999999</v>
       </c>
     </row>
     <row r="10" spans="3:18" x14ac:dyDescent="0.25">
@@ -686,11 +694,11 @@
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>119.07</v>
+        <v>198.45</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="1"/>
-        <v>184.2286761</v>
+        <v>307.04779350000001</v>
       </c>
       <c r="G10" t="s">
         <v>6</v>
@@ -705,11 +713,11 @@
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>18.899999999999999</v>
+        <v>31.499999999999996</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="1"/>
-        <v>29.242646999999998</v>
+        <v>48.737744999999997</v>
       </c>
     </row>
     <row r="12" spans="3:18" x14ac:dyDescent="0.25">
@@ -721,11 +729,11 @@
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>28.349999999999998</v>
+        <v>47.25</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="1"/>
-        <v>43.863970500000001</v>
+        <v>73.106617499999999</v>
       </c>
     </row>
     <row r="13" spans="3:18" x14ac:dyDescent="0.25">
@@ -737,11 +745,11 @@
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>11.339999999999998</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="F13" s="4">
         <f t="shared" si="1"/>
-        <v>17.545588199999997</v>
+        <v>29.242646999999998</v>
       </c>
     </row>
     <row r="14" spans="3:18" x14ac:dyDescent="0.25">
@@ -791,11 +799,11 @@
       </c>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>7.56</v>
+        <v>12.6</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" si="1"/>
-        <v>11.697058800000001</v>
+        <v>19.495098000000002</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
@@ -808,11 +816,11 @@
       </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>17.009999999999998</v>
+        <v>28.349999999999998</v>
       </c>
       <c r="F17" s="4">
         <f t="shared" si="1"/>
-        <v>26.3183823</v>
+        <v>43.863970500000001</v>
       </c>
       <c r="G17" t="s">
         <v>28</v>
@@ -827,11 +835,11 @@
       </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>28.349999999999998</v>
+        <v>47.25</v>
       </c>
       <c r="F18" s="4">
         <f t="shared" si="1"/>
-        <v>43.863970500000001</v>
+        <v>73.106617499999999</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
@@ -843,11 +851,11 @@
       </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>39.69</v>
+        <v>66.149999999999991</v>
       </c>
       <c r="F19" s="4">
         <f t="shared" si="1"/>
-        <v>61.409558699999998</v>
+        <v>102.34926449999999</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
@@ -878,11 +886,11 @@
       </c>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>34.019999999999996</v>
+        <v>56.699999999999996</v>
       </c>
       <c r="F21" s="4">
         <f t="shared" si="1"/>
-        <v>52.636764599999999</v>
+        <v>87.727941000000001</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
@@ -913,11 +921,11 @@
       </c>
       <c r="E23" s="4">
         <f t="shared" si="0"/>
-        <v>5.669999999999999</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="F23" s="4">
         <f t="shared" si="1"/>
-        <v>8.7727940999999987</v>
+        <v>14.621323499999999</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
@@ -949,11 +957,11 @@
       </c>
       <c r="E25" s="4">
         <f t="shared" si="0"/>
-        <v>32.129999999999995</v>
+        <v>53.55</v>
       </c>
       <c r="F25" s="4">
         <f t="shared" si="1"/>
-        <v>49.712499899999997</v>
+        <v>82.854166500000005</v>
       </c>
       <c r="G25" t="s">
         <v>27</v>
@@ -968,11 +976,11 @@
       </c>
       <c r="E26" s="4">
         <f t="shared" si="0"/>
-        <v>28.349999999999998</v>
+        <v>47.25</v>
       </c>
       <c r="F26" s="4">
         <f t="shared" si="1"/>
-        <v>43.863970500000001</v>
+        <v>73.106617499999999</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
@@ -984,11 +992,11 @@
       </c>
       <c r="E27" s="4">
         <f t="shared" si="0"/>
-        <v>7.56</v>
+        <v>12.6</v>
       </c>
       <c r="F27" s="4">
         <f t="shared" si="1"/>
-        <v>11.697058800000001</v>
+        <v>19.495098000000002</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
@@ -1001,11 +1009,11 @@
       </c>
       <c r="E28" s="4">
         <f t="shared" si="0"/>
-        <v>9.4499999999999993</v>
+        <v>15.749999999999998</v>
       </c>
       <c r="F28" s="4">
         <f t="shared" si="1"/>
-        <v>14.621323499999999</v>
+        <v>24.368872499999998</v>
       </c>
       <c r="G28" t="s">
         <v>36</v>
@@ -1020,11 +1028,11 @@
       </c>
       <c r="E29" s="4">
         <f t="shared" si="0"/>
-        <v>17.009999999999998</v>
+        <v>28.349999999999998</v>
       </c>
       <c r="F29" s="4">
         <f t="shared" si="1"/>
-        <v>26.3183823</v>
+        <v>43.863970500000001</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
@@ -1036,11 +1044,11 @@
       </c>
       <c r="E30" s="4">
         <f t="shared" si="0"/>
-        <v>5.669999999999999</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="F30" s="4">
         <f t="shared" si="1"/>
-        <v>8.7727940999999987</v>
+        <v>14.621323499999999</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
@@ -1088,11 +1096,11 @@
       </c>
       <c r="E33" s="4">
         <f t="shared" si="0"/>
-        <v>18.899999999999999</v>
+        <v>31.499999999999996</v>
       </c>
       <c r="F33" s="4">
         <f>E33*1.54723</f>
-        <v>29.242646999999998</v>
+        <v>48.737744999999997</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
@@ -1105,11 +1113,11 @@
       </c>
       <c r="E35" s="4" t="str">
         <f>ROUND(SUM(E5:E33),1)&amp;" MGD"</f>
-        <v>718.2 MGD</v>
+        <v>1197 MGD</v>
       </c>
       <c r="F35" s="4" t="str">
         <f>ROUND(SUM(F5:F33),1)&amp;" cfs"</f>
-        <v>1111.2 cfs</v>
+        <v>1852 cfs</v>
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Defined inlet flow rate for OSH and added catchments to VA hosp.
</commit_message>
<xml_diff>
--- a/Inlet_calculations.xlsx
+++ b/Inlet_calculations.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\modeling\HEC-HMS\Bloomingdale\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="12300"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t>loc-MM7</t>
   </si>
@@ -99,9 +104,6 @@
     <t>in-MM6</t>
   </si>
   <si>
-    <t>subtracted in-MM6</t>
-  </si>
-  <si>
     <t>subtracted in-MSF1 and in-aa3MM</t>
   </si>
   <si>
@@ -169,6 +171,15 @@
   </si>
   <si>
     <t>loc-MM2b</t>
+  </si>
+  <si>
+    <t>Assume little or no runoff based on obs, record drawings. All 3x barrel inlets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OSH Assume little or no runoff based on obs, record drawings. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OSH Includes private. Assume little or no runoff. </t>
   </si>
 </sst>
 </file>
@@ -178,7 +189,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,8 +205,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,8 +227,25 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -217,11 +253,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -232,8 +284,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -241,6 +299,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -289,7 +350,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -324,7 +385,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -535,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,67 +610,70 @@
   <sheetData>
     <row r="2" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J2" s="1">
         <v>1.5</v>
       </c>
       <c r="L2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N2" s="1">
         <v>1.8</v>
       </c>
       <c r="O2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" t="s">
         <v>44</v>
-      </c>
-      <c r="P2" t="s">
-        <v>45</v>
       </c>
       <c r="Q2" s="1">
         <v>30</v>
       </c>
       <c r="R2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="3:18" s="2" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="3:18" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    </row>
+    <row r="5" spans="3:18" s="6" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
+        <f>20</f>
         <v>20</v>
       </c>
-      <c r="E5" s="4">
-        <f>D5*$J$2*$N$2*(1-$Q$2/100)</f>
-        <v>37.799999999999997</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="E5" s="8">
+        <v>300</v>
+      </c>
+      <c r="F5" s="7">
         <f>E5*1.54723</f>
-        <v>58.485293999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
+        <v>464.16900000000004</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="3:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>11</v>
       </c>
@@ -628,7 +692,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>0</v>
       </c>
@@ -644,23 +708,25 @@
         <v>157.91029380000001</v>
       </c>
     </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+    <row r="8" spans="3:18" s="6" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>32</v>
       </c>
-      <c r="E8" s="4">
-        <f t="shared" si="0"/>
-        <v>60.48</v>
-      </c>
-      <c r="F8" s="4">
-        <f t="shared" si="1"/>
-        <v>93.576470400000005</v>
-      </c>
-    </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="E8" s="8">
+        <v>300</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="1"/>
+        <v>464.16900000000004</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="3:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>3</v>
       </c>
@@ -815,7 +881,7 @@
         <v>26.3183823</v>
       </c>
       <c r="G17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
@@ -850,7 +916,7 @@
         <v>61.409558699999998</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>19</v>
       </c>
@@ -869,23 +935,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+    <row r="21" spans="3:7" s="6" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D21">
-        <v>18</v>
-      </c>
-      <c r="E21" s="4">
-        <f t="shared" si="0"/>
-        <v>34.019999999999996</v>
-      </c>
-      <c r="F21" s="4">
-        <f t="shared" si="1"/>
-        <v>52.636764599999999</v>
-      </c>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D21" s="7">
+        <v>50</v>
+      </c>
+      <c r="E21" s="8">
+        <v>300</v>
+      </c>
+      <c r="F21" s="7">
+        <f t="shared" si="1"/>
+        <v>464.16900000000004</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>22</v>
       </c>
@@ -925,38 +993,37 @@
         <v>25</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="F24" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14.621323499999999</v>
       </c>
       <c r="G24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+    <row r="25" spans="3:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="9">
+        <v>24</v>
+      </c>
+      <c r="E25" s="10">
+        <f t="shared" si="0"/>
+        <v>45.359999999999992</v>
+      </c>
+      <c r="F25" s="10">
+        <f t="shared" si="1"/>
+        <v>70.18235279999999</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="D25">
-        <f>32-D26</f>
-        <v>17</v>
-      </c>
-      <c r="E25" s="4">
-        <f t="shared" si="0"/>
-        <v>32.129999999999995</v>
-      </c>
-      <c r="F25" s="4">
-        <f t="shared" si="1"/>
-        <v>49.712499899999997</v>
-      </c>
-      <c r="G25" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
@@ -964,20 +1031,20 @@
         <v>26</v>
       </c>
       <c r="D26">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E26" s="4">
         <f t="shared" si="0"/>
-        <v>28.349999999999998</v>
+        <v>60.48</v>
       </c>
       <c r="F26" s="4">
         <f t="shared" si="1"/>
-        <v>43.863970500000001</v>
+        <v>93.576470400000005</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D27">
         <v>4</v>
@@ -993,7 +1060,7 @@
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28">
         <f>14-D29</f>
@@ -1008,12 +1075,12 @@
         <v>14.621323499999999</v>
       </c>
       <c r="G28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29">
         <v>9</v>
@@ -1029,7 +1096,7 @@
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -1045,7 +1112,7 @@
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1061,7 +1128,7 @@
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32">
         <f>10-D33</f>
@@ -1076,12 +1143,12 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33">
         <v>10</v>
@@ -1097,19 +1164,19 @@
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D35" t="str">
         <f>SUM(D5:D33) &amp;" inlets"</f>
-        <v>380 inlets</v>
+        <v>441 inlets</v>
       </c>
       <c r="E35" s="4" t="str">
         <f>ROUND(SUM(E5:E33),1)&amp;" MGD"</f>
-        <v>718.2 MGD</v>
+        <v>1540.7 MGD</v>
       </c>
       <c r="F35" s="4" t="str">
         <f>ROUND(SUM(F5:F33),1)&amp;" cfs"</f>
-        <v>1111.2 cfs</v>
+        <v>2383.8 cfs</v>
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add inlet to McMillan. No runoff from McMillan. Base inlet count run. Using Volker's inlet counts & modified OSH, VA, and McMillan to reduce runoff from those properties.
</commit_message>
<xml_diff>
--- a/Inlet_calculations.xlsx
+++ b/Inlet_calculations.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>loc-MM7</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t xml:space="preserve">OSH Includes private. Assume little or no runoff. </t>
+  </si>
+  <si>
+    <t>McMillan. Assumed no runoff</t>
   </si>
 </sst>
 </file>
@@ -214,7 +217,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,6 +244,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -289,6 +298,9 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -596,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +822,7 @@
         <v>17.545588199999997</v>
       </c>
     </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>9</v>
       </c>
@@ -829,26 +841,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+    <row r="15" spans="3:18" s="11" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="D15" s="11">
+        <v>0</v>
+      </c>
+      <c r="E15" s="12">
+        <v>300</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" si="1"/>
+        <v>464.16900000000004</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="3:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>15</v>
       </c>
@@ -1094,7 +1105,7 @@
         <v>26.3183823</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
         <v>31</v>
       </c>
@@ -1110,23 +1121,25 @@
         <v>8.7727940999999987</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+    <row r="31" spans="3:7" s="11" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="11">
+        <v>0</v>
+      </c>
+      <c r="E31" s="12">
+        <v>300</v>
+      </c>
+      <c r="F31" s="13">
+        <f t="shared" si="1"/>
+        <v>464.16900000000004</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>33</v>
       </c>
@@ -1172,11 +1185,11 @@
       </c>
       <c r="E35" s="4" t="str">
         <f>ROUND(SUM(E5:E33),1)&amp;" MGD"</f>
-        <v>1540.7 MGD</v>
+        <v>2140.7 MGD</v>
       </c>
       <c r="F35" s="4" t="str">
         <f>ROUND(SUM(F5:F33),1)&amp;" cfs"</f>
-        <v>2383.8 cfs</v>
+        <v>3312.2 cfs</v>
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Increase barrel multiplier to 2.5
</commit_message>
<xml_diff>
--- a/Inlet_calculations.xlsx
+++ b/Inlet_calculations.xlsx
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +628,7 @@
         <v>41</v>
       </c>
       <c r="J2" s="1">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="L2" t="s">
         <v>42</v>
@@ -713,11 +713,11 @@
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>102.06</v>
+        <v>170.1</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="1"/>
-        <v>157.91029380000001</v>
+        <v>263.18382300000002</v>
       </c>
     </row>
     <row r="8" spans="3:18" s="6" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -747,11 +747,11 @@
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>88.83</v>
+        <v>148.04999999999998</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="1"/>
-        <v>137.4404409</v>
+        <v>229.06740149999999</v>
       </c>
     </row>
     <row r="10" spans="3:18" x14ac:dyDescent="0.25">
@@ -764,11 +764,11 @@
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>119.07</v>
+        <v>198.45</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="1"/>
-        <v>184.2286761</v>
+        <v>307.04779350000001</v>
       </c>
       <c r="G10" t="s">
         <v>6</v>
@@ -783,11 +783,11 @@
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>18.899999999999999</v>
+        <v>31.499999999999996</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="1"/>
-        <v>29.242646999999998</v>
+        <v>48.737744999999997</v>
       </c>
     </row>
     <row r="12" spans="3:18" x14ac:dyDescent="0.25">
@@ -799,11 +799,11 @@
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>28.349999999999998</v>
+        <v>47.25</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="1"/>
-        <v>43.863970500000001</v>
+        <v>73.106617499999999</v>
       </c>
     </row>
     <row r="13" spans="3:18" x14ac:dyDescent="0.25">
@@ -815,11 +815,11 @@
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>11.339999999999998</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="F13" s="4">
         <f t="shared" si="1"/>
-        <v>17.545588199999997</v>
+        <v>29.242646999999998</v>
       </c>
     </row>
     <row r="14" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -868,11 +868,11 @@
       </c>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>7.56</v>
+        <v>12.6</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" si="1"/>
-        <v>11.697058800000001</v>
+        <v>19.495098000000002</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
@@ -885,11 +885,11 @@
       </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>17.009999999999998</v>
+        <v>28.349999999999998</v>
       </c>
       <c r="F17" s="4">
         <f t="shared" si="1"/>
-        <v>26.3183823</v>
+        <v>43.863970500000001</v>
       </c>
       <c r="G17" t="s">
         <v>27</v>
@@ -904,11 +904,11 @@
       </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>28.349999999999998</v>
+        <v>47.25</v>
       </c>
       <c r="F18" s="4">
         <f t="shared" si="1"/>
-        <v>43.863970500000001</v>
+        <v>73.106617499999999</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
@@ -920,11 +920,11 @@
       </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>39.69</v>
+        <v>66.149999999999991</v>
       </c>
       <c r="F19" s="4">
         <f t="shared" si="1"/>
-        <v>61.409558699999998</v>
+        <v>102.34926449999999</v>
       </c>
     </row>
     <row r="20" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -992,11 +992,11 @@
       </c>
       <c r="E23" s="4">
         <f t="shared" si="0"/>
-        <v>5.669999999999999</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="F23" s="4">
         <f t="shared" si="1"/>
-        <v>8.7727940999999987</v>
+        <v>14.621323499999999</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
@@ -1008,11 +1008,11 @@
       </c>
       <c r="E24" s="4">
         <f t="shared" si="0"/>
-        <v>9.4499999999999993</v>
+        <v>15.749999999999998</v>
       </c>
       <c r="F24" s="4">
         <f t="shared" si="1"/>
-        <v>14.621323499999999</v>
+        <v>24.368872499999998</v>
       </c>
       <c r="G24" t="s">
         <v>13</v>
@@ -1027,11 +1027,11 @@
       </c>
       <c r="E25" s="10">
         <f t="shared" si="0"/>
-        <v>45.359999999999992</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="F25" s="10">
         <f t="shared" si="1"/>
-        <v>70.18235279999999</v>
+        <v>116.97058799999999</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>50</v>
@@ -1046,11 +1046,11 @@
       </c>
       <c r="E26" s="4">
         <f t="shared" si="0"/>
-        <v>60.48</v>
+        <v>100.8</v>
       </c>
       <c r="F26" s="4">
         <f t="shared" si="1"/>
-        <v>93.576470400000005</v>
+        <v>155.96078400000002</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
@@ -1062,11 +1062,11 @@
       </c>
       <c r="E27" s="4">
         <f t="shared" si="0"/>
-        <v>7.56</v>
+        <v>12.6</v>
       </c>
       <c r="F27" s="4">
         <f t="shared" si="1"/>
-        <v>11.697058800000001</v>
+        <v>19.495098000000002</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
@@ -1079,11 +1079,11 @@
       </c>
       <c r="E28" s="4">
         <f t="shared" si="0"/>
-        <v>9.4499999999999993</v>
+        <v>15.749999999999998</v>
       </c>
       <c r="F28" s="4">
         <f t="shared" si="1"/>
-        <v>14.621323499999999</v>
+        <v>24.368872499999998</v>
       </c>
       <c r="G28" t="s">
         <v>35</v>
@@ -1098,11 +1098,11 @@
       </c>
       <c r="E29" s="4">
         <f t="shared" si="0"/>
-        <v>17.009999999999998</v>
+        <v>28.349999999999998</v>
       </c>
       <c r="F29" s="4">
         <f t="shared" si="1"/>
-        <v>26.3183823</v>
+        <v>43.863970500000001</v>
       </c>
     </row>
     <row r="30" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1114,11 +1114,11 @@
       </c>
       <c r="E30" s="4">
         <f t="shared" si="0"/>
-        <v>5.669999999999999</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="F30" s="4">
         <f t="shared" si="1"/>
-        <v>8.7727940999999987</v>
+        <v>14.621323499999999</v>
       </c>
     </row>
     <row r="31" spans="3:7" s="11" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1168,11 +1168,11 @@
       </c>
       <c r="E33" s="4">
         <f t="shared" si="0"/>
-        <v>18.899999999999999</v>
+        <v>31.499999999999996</v>
       </c>
       <c r="F33" s="4">
         <f>E33*1.54723</f>
-        <v>29.242646999999998</v>
+        <v>48.737744999999997</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
@@ -1185,11 +1185,11 @@
       </c>
       <c r="E35" s="4" t="str">
         <f>ROUND(SUM(E5:E33),1)&amp;" MGD"</f>
-        <v>2140.7 MGD</v>
+        <v>2567.9 MGD</v>
       </c>
       <c r="F35" s="4" t="str">
         <f>ROUND(SUM(F5:F33),1)&amp;" cfs"</f>
-        <v>3312.2 cfs</v>
+        <v>3973.1 cfs</v>
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>